<commit_message>
Add November 22nd's blog
</commit_message>
<xml_diff>
--- a/posts/2024-11-13_motorway-service-stations-info/retailer_types.xlsx
+++ b/posts/2024-11-13_motorway-service-stations-info/retailer_types.xlsx
@@ -8,19 +8,32 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/charliejhadley/Github/visibledata.github.io/posts/2024-11-13_motorway-service-stations-info/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{5814B73C-A5F7-E84D-A693-417256841CF4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{D0FC6915-BFF6-1F47-BA29-5919CC3F0642}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="880" windowWidth="36000" windowHeight="22500" xr2:uid="{9A86607B-DD9E-F04F-9561-1E486A946F78}"/>
   </bookViews>
   <sheets>
     <sheet name="retailer_types" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="323" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="324" uniqueCount="106">
   <si>
     <t>retailer</t>
   </si>
@@ -118,10 +131,6 @@
     <t>FoneBiz</t>
   </si>
   <si>
-    <t>Food to Go
-Farm Cafe</t>
-  </si>
-  <si>
     <t>Fresh Express</t>
   </si>
   <si>
@@ -339,6 +348,9 @@
   </si>
   <si>
     <t>is_food_retailer</t>
+  </si>
+  <si>
+    <t>Food to Go - Farm Cafe</t>
   </si>
 </sst>
 </file>
@@ -1205,10 +1217,10 @@
   <dimension ref="A1:F99"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="244" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B25" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="C3" sqref="C3"/>
+      <selection pane="bottomRight" activeCell="A33" sqref="A33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1223,19 +1235,19 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C1" t="s">
+        <v>100</v>
+      </c>
+      <c r="D1" t="s">
         <v>101</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>102</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>103</v>
-      </c>
-      <c r="F1" t="s">
-        <v>104</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
@@ -1243,13 +1255,13 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
@@ -1257,10 +1269,10 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
@@ -1268,13 +1280,13 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C4" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
@@ -1282,10 +1294,10 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C5" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
@@ -1293,10 +1305,10 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C6" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
@@ -1304,10 +1316,10 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C7" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
@@ -1315,13 +1327,13 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C8" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E8" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
@@ -1329,13 +1341,13 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C9" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D9" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
@@ -1343,10 +1355,10 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C10" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
@@ -1354,16 +1366,16 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C11" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D11" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="F11" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
@@ -1371,10 +1383,10 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C12" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
@@ -1382,10 +1394,10 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C13" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
@@ -1393,13 +1405,13 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C14" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D14" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
@@ -1407,10 +1419,10 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C15" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
@@ -1418,16 +1430,16 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C16" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D16" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="F16" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
@@ -1435,16 +1447,16 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C17" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D17" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="F17" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
@@ -1452,16 +1464,16 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C18" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D18" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="F18" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
@@ -1469,16 +1481,16 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C19" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D19" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="F19" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
@@ -1486,10 +1498,10 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C20" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
@@ -1497,13 +1509,13 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C21" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D21" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
@@ -1511,13 +1523,13 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C22" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D22" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
@@ -1525,16 +1537,16 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C23" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D23" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="F23" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
@@ -1542,13 +1554,13 @@
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C24" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D24" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.2">
@@ -1556,13 +1568,13 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C25" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D25" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.2">
@@ -1570,13 +1582,13 @@
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C26" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D26" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.2">
@@ -1584,13 +1596,13 @@
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C27" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D27" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.2">
@@ -1598,13 +1610,13 @@
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C28" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D28" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.2">
@@ -1612,13 +1624,13 @@
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C29" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D29" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.2">
@@ -1626,10 +1638,13 @@
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E30" t="s">
-        <v>98</v>
+        <v>97</v>
+      </c>
+      <c r="F30" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.2">
@@ -1637,16 +1652,16 @@
         <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C31" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D31" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E31" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.2">
@@ -1654,735 +1669,735 @@
         <v>31</v>
       </c>
       <c r="B32" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
-        <v>32</v>
+        <v>105</v>
       </c>
       <c r="B33" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C33" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D33" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="F33" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B34" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C34" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D34" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B35" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C35" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D35" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="F35" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B36" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B37" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B38" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B39" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B40" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B41" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C41" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D41" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="F41" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B42" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C42" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D42" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="F42" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B43" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B44" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C44" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D44" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B45" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C45" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D45" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B46" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C46" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B47" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C47" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D47" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B48" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B49" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C49" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D49" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="F49" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B50" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B51" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B52" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C52" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D52" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="F52" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B53" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B54" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B55" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E55" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B56" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E56" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B57" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C57" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D57" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B58" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D58" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="F58" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B59" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B60" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B61" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C61" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D61" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B62" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D62" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="F62" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B63" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B64" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C64" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D64" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B65" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B66" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B67" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C67" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B68" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="F68" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B69" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B70" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D70" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="F70" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B71" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E71" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B72" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="F72" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B73" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B74" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B75" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D75" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="F75" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B76" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C76" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D76" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B77" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B78" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B79" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C79" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D79" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B80" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E80" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B81" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B82" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B83" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B84" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B85" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B86" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D86" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="F86" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B87" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B88" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E88" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B89" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E89" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B90" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B91" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="F91" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B92" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C92" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D92" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B93" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B94" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C94" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D94" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B95" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="F95" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B96" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C96" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D96" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B97" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B98" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B99" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
   </sheetData>

</xml_diff>